<commit_message>
Deploying to gh-pages from @ tech-acs/crvsreportpackage@64b63355c899022c9a6252441b349326adb0d085 🚀
</commit_message>
<xml_diff>
--- a/reference/output.xlsx
+++ b/reference/output.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="convert_csv_xlsx" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -15,8 +15,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -44,8 +52,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,12 +351,531 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>&lt;!DOCTYPE html&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>&lt;!-- Generated by pkgdown: do not edit by hand --&gt;&lt;html lang="en"&gt;&lt;head&gt;&lt;meta http-equiv="Content-Type" content="text/html; charset=UTF-8"&gt;&lt;meta charset="utf-8"&gt;&lt;meta http-equiv="X-UA-Compatible" content="IE=edge"&gt;&lt;meta name="viewport" content="width=device-width, initial-scale=1, shrink-to-fit=no"&gt;&lt;title&gt;Convert CSV Files to an Excel Workbook — convert_csv_xlsx • crvsreportpackage&lt;/title&gt;&lt;script src="../lightswitch.js"&gt;&lt;/script&gt;&lt;script src="../deps/jquery-3.6.0/jquery-3.6.0.min.js"&gt;&lt;/script&gt;&lt;meta name="viewport" content="width=device-width, initial-scale=1, shrink-to-fit=no"&gt;&lt;link href="../deps/bootstrap-5.3.1/bootstrap.min.css" rel="stylesheet"&gt;&lt;script src="../deps/bootstrap-5.3.1/bootstrap.bundle.min.js"&gt;&lt;/script&gt;&lt;link href="../deps/font-awesome-6.4.2/css/all.min.css" rel="stylesheet"&gt;&lt;link href="../deps/font-awesome-6.4.2/css/v4-shims.min.css" rel="stylesheet"&gt;&lt;script src="../deps/headroom-0.11.0/headroom.min.js"&gt;&lt;/script&gt;&lt;script src="../deps/headroom-0.11.0/jQuery.headroom.min.js"&gt;&lt;/script&gt;&lt;script src="../deps/bootstrap-toc-1.0.1/bootstrap-toc.min.js"&gt;&lt;/script&gt;&lt;script src="../deps/clipboard.js-2.0.11/clipboard.min.js"&gt;&lt;/script&gt;&lt;script src="../deps/search-1.0.0/autocomplete.jquery.min.js"&gt;&lt;/script&gt;&lt;script src="../deps/search-1.0.0/fuse.min.js"&gt;&lt;/script&gt;&lt;script src="../deps/search-1.0.0/mark.min.js"&gt;&lt;/script&gt;&lt;!-- pkgdown --&gt;&lt;script src="../pkgdown.js"&gt;&lt;/script&gt;&lt;meta property="og:title" content="Convert CSV Files to an Excel Workbook — convert_csv_xlsx"&gt;&lt;meta name="description" content="This function reads all CSV files in a specified directory and writes their contents to separate sheets in a single Excel workbook."&gt;&lt;meta property="og:description" content="This function reads all CSV files in a specified directory and writes their contents to separate sheets in a single Excel workbook."&gt;&lt;/head&gt;&lt;body&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>&lt;a href="#main" class="visually-hidden-focusable"&gt;Skip to contents&lt;/a&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>&lt;nav class="navbar navbar-expand-lg fixed-top " aria-label="Site navigation"&gt;&lt;div class="container"&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>&lt;a class="navbar-brand me-2" href="../index.html"&gt;crvsreportpackage&lt;/a&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>&lt;small class="nav-text text-muted me-auto" data-bs-toggle="tooltip" data-bs-placement="bottom" title=""&gt;0.2.3&lt;/small&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>&lt;button class="navbar-toggler" type="button" data-bs-toggle="collapse" data-bs-target="#navbar" aria-controls="navbar" aria-expanded="false" aria-label="Toggle navigation"&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>&lt;span class="navbar-toggler-icon"&gt;&lt;/span&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>&lt;/button&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>&lt;div id="navbar" class="collapse navbar-collapse ms-3"&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>&lt;ul class="navbar-nav me-auto"&gt;&lt;li class="nav-item"&gt;&lt;a class="nav-link" href="../articles/crvsreportpackage.html"&gt;Get started&lt;/a&gt;&lt;/li&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>&lt;li class="active nav-item"&gt;&lt;a class="nav-link" href="../reference/index.html"&gt;Reference&lt;/a&gt;&lt;/li&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>&lt;li class="nav-item dropdown"&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>&lt;button class="nav-link dropdown-toggle" type="button" id="dropdown-articles" data-bs-toggle="dropdown" aria-expanded="false" aria-haspopup="true"&gt;Articles&lt;/button&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>&lt;ul class="dropdown-menu" aria-labelledby="dropdown-articles"&gt;&lt;li&gt;&lt;a class="dropdown-item" href="../articles/data_cleaning.html"&gt;Data cleaning&lt;/a&gt;&lt;/li&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>&lt;li&gt;&lt;a class="dropdown-item" href="../articles/data_mapping.html"&gt;Mapping variables to CRVS tables and figures&lt;/a&gt;&lt;/li&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>&lt;li&gt;&lt;a class="dropdown-item" href="../articles/table_templates.html"&gt;CRVS tables&lt;/a&gt;&lt;/li&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>&lt;/ul&gt;&lt;/li&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>&lt;/ul&gt;&lt;ul class="navbar-nav"&gt;&lt;li class="nav-item"&gt;&lt;form class="form-inline" role="search"&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>&lt;input class="form-control" type="search" name="search-input" id="search-input" autocomplete="off" aria-label="Search site" placeholder="Search for" data-search-index="../search.json"&gt;&lt;/form&gt;&lt;/li&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>&lt;li class="nav-item dropdown"&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>&lt;button class="nav-link dropdown-toggle" type="button" id="dropdown-lightswitch" data-bs-toggle="dropdown" aria-expanded="false" aria-haspopup="true" aria-label="Light switch"&gt;&lt;span class="fa fa-sun"&gt;&lt;/span&gt;&lt;/button&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>&lt;ul class="dropdown-menu dropdown-menu-end" aria-labelledby="dropdown-lightswitch"&gt;&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="light"&gt;&lt;span class="fa fa-sun"&gt;&lt;/span&gt; Light&lt;/button&gt;&lt;/li&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="dark"&gt;&lt;span class="fa fa-moon"&gt;&lt;/span&gt; Dark&lt;/button&gt;&lt;/li&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>&lt;li&gt;&lt;button class="dropdown-item" data-bs-theme-value="auto"&gt;&lt;span class="fa fa-adjust"&gt;&lt;/span&gt; Auto&lt;/button&gt;&lt;/li&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>&lt;/ul&gt;&lt;/li&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>&lt;/ul&gt;&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>&lt;/nav&gt;&lt;div class="container template-reference-topic"&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>&lt;div class="row"&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>&lt;main id="main" class="col-md-9"&gt;&lt;div class="page-header"&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>&lt;h1&gt;Convert CSV Files to an Excel Workbook&lt;/h1&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>&lt;div class="d-none name"&gt;&lt;code&gt;convert_csv_xlsx.Rd&lt;/code&gt;&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>&lt;div class="ref-description section level2"&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;This function reads all CSV files in a specified directory and writes their contents to separate sheets in a single Excel workbook.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>&lt;div class="section level2"&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>&lt;h2 id="ref-usage"&gt;Usage&lt;a class="anchor" aria-label="anchor" href="#ref-usage"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>&lt;div class="sourceCode"&gt;&lt;pre class="sourceCode r"&gt;&lt;code&gt;&lt;span&gt;&lt;span class="fu"&gt;convert_csv_xlsx&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;input_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"."&lt;/span&gt;, output_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"output.xlsx"&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>&lt;div class="section level2"&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>&lt;h2 id="arguments"&gt;Arguments&lt;a class="anchor" aria-label="anchor" href="#arguments"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>&lt;dl&gt;&lt;dt id="arg-output-path"&gt;output_path&lt;a class="anchor" aria-label="anchor" href="#arg-output-path"&gt;&lt;/a&gt;&lt;/dt&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>&lt;dd&gt;&lt;p&gt;A character string specifying the directory and file name to write the xlsx to.&lt;/p&gt;&lt;/dd&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>&lt;dt id="arg-path"&gt;path&lt;a class="anchor" aria-label="anchor" href="#arg-path"&gt;&lt;/a&gt;&lt;/dt&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>&lt;dd&gt;&lt;p&gt;A character string specifying the directory containing the CSV files. Defaults to the current working directory (".").&lt;/p&gt;&lt;/dd&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>&lt;/dl&gt;&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>&lt;div class="section level2"&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>&lt;h2 id="value"&gt;Value&lt;a class="anchor" aria-label="anchor" href="#value"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;An Excel file named "output.xlsx" containing the contents of the CSV files.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>&lt;div class="section level2"&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>&lt;h2 id="ref-examples"&gt;Examples&lt;a class="anchor" aria-label="anchor" href="#ref-examples"&gt;&lt;/a&gt;&lt;/h2&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>&lt;div class="sourceCode"&gt;&lt;pre class="sourceCode r"&gt;&lt;code&gt;&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="co"&gt;# Convert CSV files in the current directory to an Excel workbook&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="fu"&gt;&lt;a href="csv_to_excel.html"&gt;csv_to_excel&lt;/a&gt;&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"."&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>&lt;span class="r-wrn co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; &lt;span class="warning"&gt;Warning: &lt;/span&gt;There are no .csv files in this directory&lt;/span&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>&lt;span class="r-out co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; NULL&lt;/span&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="co"&gt;# Convert CSV files in a specified directory to an Excel workbook&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>&lt;span class="r-in"&gt;&lt;span&gt;&lt;span class="fu"&gt;&lt;a href="csv_to_excel.html"&gt;csv_to_excel&lt;/a&gt;&lt;/span&gt;&lt;span class="op"&gt;(&lt;/span&gt;input_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"path/to/directory"&lt;/span&gt;, output_path &lt;span class="op"&gt;=&lt;/span&gt; &lt;span class="st"&gt;"path/with/file/output.xlsx"&lt;/span&gt;&lt;span class="op"&gt;)&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>&lt;span class="r-err co"&gt;&lt;span class="r-pr"&gt;#&amp;gt;&lt;/span&gt; &lt;span class="error"&gt;Error in csv_to_excel(input_path = "path/to/directory", output_path = "path/with/file/output.xlsx"):&lt;/span&gt; unused arguments (input_path = "path/to/directory", output_path = "path/with/file/output.xlsx")&lt;/span&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>&lt;/code&gt;&lt;/pre&gt;&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>&lt;/main&gt;&lt;aside class="col-md-3"&gt;&lt;nav id="toc" aria-label="Table of contents"&gt;&lt;h2&gt;On this page&lt;/h2&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>&lt;/nav&gt;&lt;/aside&gt;&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>&lt;footer&gt;&lt;div class="pkgdown-footer-left"&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Developed by Tesfaye Belay, Pamela Kakande, Rachel Shipsey, Liam Beardsmore.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>&lt;div class="pkgdown-footer-right"&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Site built with &lt;a href="https://pkgdown.r-lib.org/" class="external-link"&gt;pkgdown&lt;/a&gt; 2.1.0.&lt;/p&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>&lt;/footer&gt;&lt;/div&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>&lt;/body&gt;&lt;/html&gt;</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>